<commit_message>
samples: wifi: thread_coex: Initial skeleton version
NRF700X_BT_COEX replaced with NRF700X_SR_COEX in driver.
Already present in sample but missing in the driver.

ToDo: Start adding Thread CLI related function calls.

Signed-off-by: Murali Thokala <Murali.Thokala@nordicsemi.no>
</commit_message>
<xml_diff>
--- a/samples/wifi/thread_coex/todo.xlsx
+++ b/samples/wifi/thread_coex/todo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\wifi_thread_coex_sample\nrf\samples\wifi\thread_coex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373B730E-1914-44FA-B348-2A5D4CCC1B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B896A3-E6ED-42F3-A3F9-D32052416138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Wi-Fi and Thread coexistence sample</t>
   </si>
@@ -105,13 +105,19 @@
   </si>
   <si>
     <t xml:space="preserve">                in R:\wifi_thread_coex_sample\nrf\samples\wifi\thread_coex\test\Kconfig</t>
+  </si>
+  <si>
+    <t>Build command</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,13 +125,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -151,6 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K24"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,17 +576,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="C18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -573,30 +597,36 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="1">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="1">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B26" s="1">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>